<commit_message>
added EM microchip data
EM microchip in database, and respective datasheets. incomplete, some datasheets are missing from their own site, either because products are too old and datasheets no longer available, or for some others where data entered is incomplete, products might be too new and datasheets not publicly available.
</commit_message>
<xml_diff>
--- a/UHF RFID tags and chips.xlsx
+++ b/UHF RFID tags and chips.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="291">
   <si>
     <t>IMPINJ</t>
   </si>
@@ -533,9 +533,6 @@
   </si>
   <si>
     <t>E200 6806</t>
-  </si>
-  <si>
-    <t>EM Microelectronic</t>
   </si>
   <si>
     <t>abbreviation</t>
@@ -884,12 +881,203 @@
   <si>
     <t>Checkpoint systems</t>
   </si>
+  <si>
+    <t>em | echo-V (EM4425)</t>
+  </si>
+  <si>
+    <t>EM4124</t>
+  </si>
+  <si>
+    <t>Read/Write, EPC Gen2 / ISO 18000-63 Type C Passive RFID IC</t>
+  </si>
+  <si>
+    <t>EM4325</t>
+  </si>
+  <si>
+    <t>EM4126</t>
+  </si>
+  <si>
+    <t>em | echo-T</t>
+  </si>
+  <si>
+    <t>Tamper-evident dual frequency RAINFC transponder IC</t>
+  </si>
+  <si>
+    <t>em | aura-C (EM4227)</t>
+  </si>
+  <si>
+    <t>RAIN RFID Crypto Transponder IC</t>
+  </si>
+  <si>
+    <t>em | echo (EM4423)</t>
+  </si>
+  <si>
+    <t>Dual Frequency RAINFC Transponder IC</t>
+  </si>
+  <si>
+    <t>em | aura-air (EM4018)</t>
+  </si>
+  <si>
+    <t>em | aura-sense (EM4152)</t>
+  </si>
+  <si>
+    <t>RAIN RFID Sensor Transponder IC</t>
+  </si>
+  <si>
+    <t>no longer available, so no datasheet for info… replaced by echo-V</t>
+  </si>
+  <si>
+    <t>-18 dBm</t>
+  </si>
+  <si>
+    <t>-12.5 dBm</t>
+  </si>
+  <si>
+    <t>2048 bits</t>
+  </si>
+  <si>
+    <t>RAINFC Authenticity Transponder IC - NFC/HF +UHF frequencies</t>
+  </si>
+  <si>
+    <t>96 bits (64 bit UID (HF))</t>
+  </si>
+  <si>
+    <t>-19 dBm IC
+-21 dBm tag</t>
+  </si>
+  <si>
+    <t>176 bits</t>
+  </si>
+  <si>
+    <t>352 bits</t>
+  </si>
+  <si>
+    <t>3072 bits</t>
+  </si>
+  <si>
+    <t>4096 bits</t>
+  </si>
+  <si>
+    <t>4 kbit Read/Write, EPC Gen2 and TOTAL / ISO 18000-63 (Gen2) and ISO 18000-64 (TOTAL) Passive or Battery-Assisted Passive RFID IC, temerature monitoring, external power output, alarm indicators, piezo interrupt</t>
+  </si>
+  <si>
+    <t>see page 18 on datasheet</t>
+  </si>
+  <si>
+    <t>208 bits</t>
+  </si>
+  <si>
+    <r>
+      <t>E200 B080</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>****</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>E200 B0C0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>****</t>
+    </r>
+  </si>
+  <si>
+    <t>**** these are 'standard configuration' TIDs. EM 4124 and 4126 reserve three bits for customer versions towards the end of the TID</t>
+  </si>
+  <si>
+    <t>0 bits</t>
+  </si>
+  <si>
+    <t>32/48/96 bits</t>
+  </si>
+  <si>
+    <t>-31 to -17, BAP</t>
+  </si>
+  <si>
+    <t>1984 bits</t>
+  </si>
+  <si>
+    <t>Fully integrated rain RFID transponder (IC+antenna)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>-18 dBm
+-16 w Psense</t>
+  </si>
+  <si>
+    <t>-13.5 dBm
+-16 w Psense</t>
+  </si>
+  <si>
+    <r>
+      <t>E280 B120</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*****</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+E280 B121
+E280 B122
+E280 B123</t>
+    </r>
+  </si>
+  <si>
+    <t>***** last two bits are TID options for taper detection (E) and PC word definition (F)</t>
+  </si>
+  <si>
+    <t>32 bits ?</t>
+  </si>
+  <si>
+    <t>416 bits</t>
+  </si>
+  <si>
+    <t>-18.5 dBm</t>
+  </si>
+  <si>
+    <t>-15.5 dBm</t>
+  </si>
+  <si>
+    <t>6 crypto keys - 1280 bits
+2 crypto keys - 1792 bits</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -954,13 +1142,27 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="35">
@@ -1354,7 +1556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1389,9 +1591,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1444,9 +1643,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
@@ -1482,6 +1678,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1522,9 +1721,6 @@
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1603,6 +1799,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1618,6 +1817,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1634,6 +1836,49 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2007,7 +2252,7 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2019,7 +2264,7 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
+      <c r="A3" s="50"/>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2029,7 +2274,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -2039,7 +2284,7 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="52" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2051,7 +2296,7 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2061,7 +2306,7 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2071,7 +2316,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2085,7 +2330,7 @@
         <v>75</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2114,10 +2359,10 @@
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="98" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>244</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2134,7 +2379,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="100" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2156,24 +2401,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD75"/>
+  <dimension ref="A1:AD68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="11" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" style="11" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="20" style="11" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="11" customWidth="1"/>
     <col min="9" max="9" width="9" style="11" customWidth="1"/>
-    <col min="10" max="11" width="13.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="11" customWidth="1"/>
     <col min="12" max="12" width="12" style="11" customWidth="1"/>
     <col min="13" max="15" width="11.42578125" style="11" customWidth="1"/>
     <col min="16" max="16" width="5.140625" customWidth="1"/>
@@ -2183,116 +2429,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="103" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="34"/>
+    </row>
+    <row r="2" spans="1:30" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" s="36"/>
-    </row>
-    <row r="2" spans="1:30" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="H2" s="21" t="s">
+      <c r="G2" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="68" t="s">
+      <c r="K2" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="70" t="s">
+      <c r="P2" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="R2" s="65" t="s">
+      <c r="R2" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
     </row>
     <row r="3" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
+      <c r="A3" s="61"/>
       <c r="B3" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>19</v>
@@ -2313,34 +2559,34 @@
       <c r="J3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="56"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="71"/>
-      <c r="R3" s="65" t="s">
+      <c r="P3" s="69"/>
+      <c r="R3" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
     </row>
     <row r="4" spans="1:30" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>20</v>
@@ -2359,31 +2605,31 @@
       <c r="J4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="56"/>
+      <c r="K4" s="55"/>
       <c r="L4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="40" t="s">
+      <c r="M4" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="O4" s="41" t="s">
+      <c r="O4" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="71"/>
-      <c r="R4" s="43" t="s">
+      <c r="P4" s="69"/>
+      <c r="R4" s="41" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>21</v>
@@ -2395,7 +2641,7 @@
         <v>29</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>31</v>
@@ -2406,371 +2652,371 @@
       <c r="J5" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="K5" s="56"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="40" t="s">
+      <c r="M5" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="O5" s="41" t="s">
+      <c r="O5" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="71"/>
+      <c r="P5" s="69"/>
     </row>
     <row r="6" spans="1:30" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="67"/>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="65"/>
+      <c r="B6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="C6" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="25"/>
+      <c r="H6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="K6" s="67"/>
+      <c r="L6" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="N6" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="P6" s="70"/>
+    </row>
+    <row r="7" spans="1:30" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="103" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="75"/>
+    </row>
+    <row r="8" spans="1:30" ht="34.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>235</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>236</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="93" t="s">
+        <v>233</v>
+      </c>
+      <c r="N8" s="93" t="s">
+        <v>234</v>
+      </c>
+      <c r="O8" s="28"/>
+      <c r="P8" s="89" t="s">
         <v>214</v>
       </c>
-      <c r="J6" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="K6" s="69"/>
-      <c r="L6" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="49" t="s">
-        <v>212</v>
-      </c>
-      <c r="N6" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="O6" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="P6" s="72"/>
-    </row>
-    <row r="7" spans="1:30" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="P7" s="77"/>
-    </row>
-    <row r="8" spans="1:30" ht="34.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="73" t="s">
-        <v>236</v>
-      </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="I8" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="94" t="s">
-        <v>234</v>
-      </c>
-      <c r="N8" s="94" t="s">
-        <v>235</v>
-      </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="90" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q8" s="81" t="s">
-        <v>221</v>
-      </c>
-      <c r="R8" s="93" t="s">
-        <v>232</v>
+      <c r="Q8" s="79" t="s">
+        <v>220</v>
+      </c>
+      <c r="R8" s="92" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="74"/>
+      <c r="D9" s="72"/>
       <c r="F9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="48" t="s">
-        <v>238</v>
+      <c r="G9" s="46" t="s">
+        <v>237</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="46" t="s">
+      <c r="I9" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="94" t="s">
+      <c r="M9" s="93" t="s">
+        <v>233</v>
+      </c>
+      <c r="N9" s="93" t="s">
         <v>234</v>
       </c>
-      <c r="N9" s="94" t="s">
-        <v>235</v>
-      </c>
-      <c r="O9" s="30"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="82"/>
-      <c r="R9" s="93"/>
-      <c r="AC9" s="38"/>
-      <c r="AD9" s="38"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="92"/>
+      <c r="AC9" s="36"/>
+      <c r="AD9" s="36"/>
     </row>
     <row r="10" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="48" t="s">
+      <c r="A10" s="61"/>
+      <c r="B10" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48" t="s">
+      <c r="E10" s="46"/>
+      <c r="F10" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I10" s="46" t="s">
+      <c r="H10" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="M10" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="N10" s="84"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="91"/>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="93"/>
+      <c r="M10" s="81" t="s">
+        <v>229</v>
+      </c>
+      <c r="N10" s="82"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="90"/>
+      <c r="Q10" s="80"/>
+      <c r="R10" s="92"/>
       <c r="S10" s="8"/>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
+      <c r="AC10" s="36"/>
+      <c r="AD10" s="36"/>
     </row>
     <row r="11" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
-      <c r="B11" s="48" t="s">
+      <c r="A11" s="61"/>
+      <c r="B11" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="46" t="s">
         <v>94</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="G11" s="48" t="s">
+      <c r="E11" s="46"/>
+      <c r="F11" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="H11" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="46" t="s">
+      <c r="H11" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="85"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="91"/>
-      <c r="Q11" s="82"/>
-      <c r="R11" s="93"/>
+      <c r="M11" s="83"/>
+      <c r="N11" s="84"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="90"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="92"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
-      <c r="B12" s="48" t="s">
+      <c r="A12" s="61"/>
+      <c r="B12" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="46" t="s">
         <v>80</v>
       </c>
       <c r="D12" s="13"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48" t="s">
+      <c r="E12" s="46"/>
+      <c r="F12" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="48" t="s">
+      <c r="G12" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" s="46" t="s">
+      <c r="H12" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="M12" s="85"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="91"/>
-      <c r="Q12" s="82"/>
-      <c r="R12" s="93"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="84"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="90"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="92"/>
     </row>
     <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="61"/>
+      <c r="B13" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="46" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48" t="s">
+      <c r="E13" s="46"/>
+      <c r="F13" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="48" t="s">
+      <c r="G13" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I13" s="46" t="s">
+      <c r="H13" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="91"/>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="93"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="90"/>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="92"/>
     </row>
     <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
-      <c r="B14" s="48" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="46" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="48" t="s">
+      <c r="H14" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="N14" s="74" t="s">
         <v>241</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="I14" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="76" t="s">
-        <v>223</v>
-      </c>
-      <c r="N14" s="76" t="s">
-        <v>242</v>
-      </c>
-      <c r="O14" s="30"/>
-      <c r="P14" s="91"/>
-      <c r="Q14" s="82"/>
-      <c r="R14" s="93"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="80"/>
+      <c r="R14" s="92"/>
     </row>
     <row r="15" spans="1:30" s="8" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="13" t="s">
         <v>43</v>
       </c>
@@ -2781,7 +3027,7 @@
         <v>55</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="46" t="s">
         <v>77</v>
       </c>
       <c r="G15" s="13" t="s">
@@ -2798,20 +3044,20 @@
       </c>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="76" t="s">
-        <v>223</v>
-      </c>
-      <c r="N15" s="76" t="s">
-        <v>229</v>
-      </c>
-      <c r="O15" s="37"/>
-      <c r="P15" s="91"/>
-      <c r="Q15" s="82"/>
-      <c r="R15" s="93"/>
+      <c r="M15" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="N15" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="O15" s="35"/>
+      <c r="P15" s="90"/>
+      <c r="Q15" s="80"/>
+      <c r="R15" s="92"/>
       <c r="S15"/>
     </row>
     <row r="16" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="11" t="s">
         <v>107</v>
       </c>
@@ -2822,31 +3068,31 @@
       <c r="F16" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="80" t="s">
-        <v>231</v>
-      </c>
-      <c r="H16" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" s="46" t="s">
+      <c r="G16" s="78" t="s">
+        <v>230</v>
+      </c>
+      <c r="H16" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J16" s="11">
         <v>0</v>
       </c>
-      <c r="M16" s="76" t="s">
-        <v>223</v>
-      </c>
-      <c r="N16" s="76" t="s">
+      <c r="M16" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="O16" s="30"/>
-      <c r="P16" s="91"/>
-      <c r="Q16" s="82"/>
-      <c r="R16" s="93"/>
+      <c r="N16" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="O16" s="29"/>
+      <c r="P16" s="90"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="92"/>
     </row>
     <row r="17" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
+      <c r="A17" s="61"/>
       <c r="B17" s="11" t="s">
         <v>106</v>
       </c>
@@ -2857,8 +3103,8 @@
       <c r="F17" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="89" t="s">
-        <v>231</v>
+      <c r="G17" s="87" t="s">
+        <v>230</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>77</v>
@@ -2869,19 +3115,19 @@
       <c r="J17" s="11">
         <v>0</v>
       </c>
-      <c r="M17" s="76" t="s">
-        <v>223</v>
-      </c>
-      <c r="N17" s="76" t="s">
+      <c r="M17" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="O17" s="30"/>
-      <c r="P17" s="91"/>
-      <c r="Q17" s="82"/>
-      <c r="R17" s="93"/>
+      <c r="N17" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="O17" s="29"/>
+      <c r="P17" s="90"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="92"/>
     </row>
     <row r="18" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
+      <c r="A18" s="61"/>
       <c r="B18" s="11" t="s">
         <v>105</v>
       </c>
@@ -2904,26 +3150,26 @@
       <c r="J18" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="M18" s="76" t="s">
-        <v>223</v>
-      </c>
-      <c r="N18" s="76" t="s">
+      <c r="M18" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="O18" s="30"/>
-      <c r="P18" s="91"/>
-      <c r="Q18" s="82"/>
-      <c r="R18" s="93"/>
+      <c r="N18" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="O18" s="29"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="92"/>
     </row>
     <row r="19" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
-      <c r="B19" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="C19" s="39" t="s">
+      <c r="A19" s="61"/>
+      <c r="B19" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="71" t="s">
         <v>54</v>
       </c>
       <c r="F19" s="11" t="s">
@@ -2941,28 +3187,28 @@
       <c r="J19" s="11">
         <v>0</v>
       </c>
-      <c r="L19" s="76"/>
-      <c r="M19" s="76" t="s">
-        <v>224</v>
-      </c>
-      <c r="N19" s="76" t="s">
-        <v>228</v>
-      </c>
-      <c r="O19" s="30"/>
-      <c r="P19" s="91"/>
-      <c r="Q19" s="82"/>
-      <c r="R19" s="93"/>
-      <c r="S19" s="38"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="N19" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="O19" s="29"/>
+      <c r="P19" s="90"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="92"/>
+      <c r="S19" s="36"/>
     </row>
     <row r="20" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="39" t="s">
+      <c r="A20" s="61"/>
+      <c r="B20" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="74"/>
+      <c r="D20" s="72"/>
       <c r="F20" s="11" t="s">
         <v>77</v>
       </c>
@@ -2978,300 +3224,300 @@
       <c r="J20" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="M20" s="76" t="s">
-        <v>224</v>
-      </c>
-      <c r="N20" s="76" t="s">
-        <v>228</v>
-      </c>
-      <c r="O20" s="30"/>
-      <c r="P20" s="91"/>
-      <c r="Q20" s="82"/>
-      <c r="R20" s="93"/>
-      <c r="S20" s="38"/>
+      <c r="M20" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="N20" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="O20" s="29"/>
+      <c r="P20" s="90"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="92"/>
+      <c r="S20" s="36"/>
     </row>
     <row r="21" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
-      <c r="B21" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" s="39" t="s">
+      <c r="A21" s="61"/>
+      <c r="B21" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="74"/>
+      <c r="D21" s="72"/>
       <c r="F21" s="11" t="s">
         <v>28</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I21" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="H21" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="M21" s="76" t="s">
-        <v>224</v>
-      </c>
-      <c r="N21" s="76" t="s">
-        <v>228</v>
-      </c>
-      <c r="O21" s="30"/>
-      <c r="P21" s="91"/>
-      <c r="Q21" s="82"/>
-      <c r="R21" s="93"/>
-      <c r="S21" s="38"/>
+      <c r="M21" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="N21" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="O21" s="29"/>
+      <c r="P21" s="90"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="92"/>
+      <c r="S21" s="36"/>
     </row>
     <row r="22" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
-      <c r="B22" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="39" t="s">
+      <c r="A22" s="61"/>
+      <c r="B22" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="74"/>
+      <c r="D22" s="72"/>
       <c r="F22" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="48" t="s">
-        <v>217</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I22" s="46" t="s">
+      <c r="G22" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="H22" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I22" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="M22" s="76" t="s">
-        <v>224</v>
-      </c>
-      <c r="N22" s="76" t="s">
-        <v>228</v>
-      </c>
-      <c r="O22" s="30"/>
-      <c r="P22" s="91"/>
-      <c r="Q22" s="82"/>
-      <c r="R22" s="93"/>
-      <c r="S22" s="38"/>
+      <c r="M22" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="N22" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="O22" s="29"/>
+      <c r="P22" s="90"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="92"/>
+      <c r="S22" s="36"/>
     </row>
     <row r="23" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
+      <c r="A23" s="61"/>
       <c r="B23" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="73" t="s">
+      <c r="D23" s="71" t="s">
         <v>46</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G23" s="48" t="s">
-        <v>218</v>
-      </c>
-      <c r="H23" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I23" s="46" t="s">
+      <c r="G23" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="H23" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J23" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M23" s="76" t="s">
-        <v>225</v>
-      </c>
-      <c r="N23" s="76" t="s">
-        <v>227</v>
-      </c>
-      <c r="O23" s="30"/>
-      <c r="P23" s="91"/>
-      <c r="Q23" s="82"/>
-      <c r="R23" s="93"/>
-      <c r="S23" s="38"/>
+      <c r="M23" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="N23" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="O23" s="29"/>
+      <c r="P23" s="90"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="92"/>
+      <c r="S23" s="36"/>
     </row>
     <row r="24" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
+      <c r="A24" s="61"/>
       <c r="B24" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="75"/>
+      <c r="D24" s="73"/>
       <c r="F24" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="79" t="s">
-        <v>219</v>
-      </c>
-      <c r="H24" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24" s="46" t="s">
+      <c r="G24" s="77" t="s">
+        <v>218</v>
+      </c>
+      <c r="H24" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="M24" s="76" t="s">
-        <v>225</v>
-      </c>
-      <c r="N24" s="76" t="s">
-        <v>227</v>
-      </c>
-      <c r="O24" s="30"/>
-      <c r="P24" s="91"/>
-      <c r="Q24" s="82"/>
-      <c r="R24" s="93"/>
-      <c r="S24" s="38"/>
+      <c r="M24" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="N24" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="O24" s="29"/>
+      <c r="P24" s="90"/>
+      <c r="Q24" s="80"/>
+      <c r="R24" s="92"/>
+      <c r="S24" s="36"/>
     </row>
     <row r="25" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="59" t="s">
+      <c r="D25" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="48" t="s">
+      <c r="F25" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="80" t="s">
-        <v>220</v>
-      </c>
-      <c r="H25" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I25" s="46" t="s">
+      <c r="G25" s="78" t="s">
+        <v>219</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" s="44" t="s">
         <v>31</v>
       </c>
       <c r="J25" s="11">
         <v>0</v>
       </c>
-      <c r="M25" s="76" t="s">
-        <v>226</v>
-      </c>
-      <c r="N25" s="76" t="s">
-        <v>223</v>
-      </c>
-      <c r="O25" s="30"/>
-      <c r="P25" s="91"/>
-      <c r="Q25" s="82"/>
-      <c r="R25" s="93"/>
-      <c r="S25" s="38"/>
+      <c r="M25" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="N25" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="O25" s="29"/>
+      <c r="P25" s="90"/>
+      <c r="Q25" s="80"/>
+      <c r="R25" s="92"/>
+      <c r="S25" s="36"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
-      <c r="B26" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="C26" s="31" t="s">
+      <c r="A26" s="65"/>
+      <c r="B26" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="66"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="G26" s="78" t="s">
-        <v>220</v>
-      </c>
-      <c r="H26" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="I26" s="46" t="s">
+      <c r="D26" s="64"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="76" t="s">
+        <v>219</v>
+      </c>
+      <c r="H26" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="31" t="s">
+      <c r="J26" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="76" t="s">
-        <v>226</v>
-      </c>
-      <c r="N26" s="76" t="s">
-        <v>223</v>
-      </c>
-      <c r="O26" s="32"/>
-      <c r="P26" s="92"/>
-      <c r="Q26" s="82"/>
-      <c r="R26" s="93"/>
-      <c r="S26" s="38"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="N26" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="O26" s="31"/>
+      <c r="P26" s="91"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="92"/>
+      <c r="S26" s="36"/>
     </row>
     <row r="27" spans="1:19" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="D27" s="18" t="s">
+      <c r="C27" s="103" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="H27" s="18" t="s">
+      <c r="G27" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="H27" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="J27" s="18" t="s">
+      <c r="J27" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L27" s="18" t="s">
+      <c r="L27" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="M27" s="18" t="s">
+      <c r="M27" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="N27" s="18" t="s">
+      <c r="N27" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="O27" s="19" t="s">
+      <c r="O27" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="60" t="s">
         <v>75</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
       <c r="F28" s="11" t="s">
         <v>102</v>
       </c>
@@ -3281,25 +3527,25 @@
       <c r="H28" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I28" s="28" t="s">
+      <c r="I28" s="27" t="s">
         <v>31</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="29"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="28"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="11" t="s">
         <v>113</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D29" s="13"/>
       <c r="F29" s="11" t="s">
@@ -3317,15 +3563,15 @@
       <c r="J29" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="O29" s="30"/>
+      <c r="O29" s="29"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="11" t="s">
         <v>115</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D30" s="13"/>
       <c r="F30" s="11" t="s">
@@ -3343,10 +3589,10 @@
       <c r="J30" s="7">
         <v>0</v>
       </c>
-      <c r="O30" s="30"/>
+      <c r="O30" s="29"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="11" t="s">
         <v>117</v>
       </c>
@@ -3358,7 +3604,7 @@
         <v>28</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>77</v>
@@ -3369,45 +3615,45 @@
       <c r="J31" s="7">
         <v>0</v>
       </c>
-      <c r="O31" s="30"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
+      <c r="A32" s="61"/>
       <c r="B32" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>173</v>
       </c>
       <c r="D32" s="13"/>
       <c r="F32" s="11" t="s">
         <v>28</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="I32" s="44" t="s">
+      <c r="I32" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="J32" s="44" t="s">
+      <c r="J32" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="O32" s="30"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
+      <c r="O32" s="29"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A33" s="61"/>
       <c r="B33" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>118</v>
       </c>
       <c r="D33" s="13"/>
       <c r="F33" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>119</v>
@@ -3419,21 +3665,21 @@
         <v>31</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="O33" s="30"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
+        <v>189</v>
+      </c>
+      <c r="O33" s="29"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A34" s="61"/>
       <c r="B34" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>120</v>
       </c>
       <c r="D34" s="9"/>
       <c r="F34" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>121</v>
@@ -3445,14 +3691,14 @@
         <v>31</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="O34" s="30"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="62"/>
+        <v>190</v>
+      </c>
+      <c r="O34" s="29"/>
+    </row>
+    <row r="35" spans="1:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="61"/>
       <c r="B35" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>122</v>
@@ -3460,7 +3706,7 @@
       <c r="D35" s="10"/>
       <c r="E35" s="13"/>
       <c r="F35" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>123</v>
@@ -3472,16 +3718,17 @@
         <v>31</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
-      <c r="O35" s="37"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
+      <c r="O35" s="35"/>
+      <c r="X35" s="102"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A36" s="61"/>
       <c r="B36" s="11" t="s">
         <v>125</v>
       </c>
@@ -3504,36 +3751,36 @@
       <c r="J36" s="7">
         <v>0</v>
       </c>
-      <c r="O36" s="30"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="62"/>
+      <c r="O36" s="29"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A37" s="61"/>
       <c r="B37" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="D37" s="43"/>
+      <c r="F37" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D37" s="45"/>
-      <c r="F37" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="H37" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="I37" s="44" t="s">
+      <c r="I37" s="42" t="s">
         <v>31</v>
       </c>
       <c r="J37" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="O37" s="30"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="62"/>
+      <c r="O37" s="29"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A38" s="61"/>
       <c r="B38" s="11" t="s">
         <v>128</v>
       </c>
@@ -3556,72 +3803,72 @@
       <c r="J38" s="7">
         <v>0</v>
       </c>
-      <c r="O38" s="30"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="62"/>
-      <c r="B39" s="58" t="s">
+      <c r="O38" s="29"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A39" s="61"/>
+      <c r="B39" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="C39" s="56" t="s">
         <v>205</v>
       </c>
-      <c r="C39" s="57" t="s">
-        <v>206</v>
-      </c>
-      <c r="D39" s="45"/>
+      <c r="D39" s="43"/>
       <c r="F39" s="11" t="s">
         <v>28</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H39" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="I39" s="56" t="s">
+      <c r="H39" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="I39" s="55" t="s">
         <v>31</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="O39" s="30"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="62"/>
-      <c r="B40" s="58"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="45"/>
+        <v>206</v>
+      </c>
+      <c r="O39" s="29"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A40" s="61"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="43"/>
       <c r="F40" s="11" t="s">
         <v>102</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H40" s="57"/>
-      <c r="I40" s="56"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="55"/>
       <c r="J40" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="O40" s="30"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="62"/>
-      <c r="B41" s="58"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="45"/>
+        <v>207</v>
+      </c>
+      <c r="O40" s="29"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A41" s="61"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="43"/>
       <c r="F41" s="11" t="s">
         <v>104</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H41" s="57"/>
-      <c r="I41" s="56"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="55"/>
       <c r="J41" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="O41" s="30"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="62"/>
+        <v>208</v>
+      </c>
+      <c r="O41" s="29"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A42" s="61"/>
       <c r="B42" s="11" t="s">
         <v>131</v>
       </c>
@@ -3630,7 +3877,7 @@
       </c>
       <c r="D42" s="10"/>
       <c r="F42" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>132</v>
@@ -3642,21 +3889,21 @@
         <v>31</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="O42" s="30"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="62"/>
-      <c r="B43" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="O42" s="29"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A43" s="61"/>
+      <c r="B43" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="42"/>
+      <c r="D43" s="40"/>
       <c r="F43" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>61</v>
@@ -3666,21 +3913,21 @@
       </c>
       <c r="I43" s="12"/>
       <c r="J43" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="O43" s="30"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="62"/>
-      <c r="B44" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="O43" s="29"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A44" s="61"/>
+      <c r="B44" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C44" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="42"/>
+      <c r="D44" s="40"/>
       <c r="F44" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G44" s="7"/>
       <c r="H44" s="11" t="s">
@@ -3689,19 +3936,19 @@
       <c r="J44" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="O44" s="30"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="62"/>
-      <c r="B45" s="39" t="s">
+      <c r="O44" s="29"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A45" s="61"/>
+      <c r="B45" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="39" t="s">
+      <c r="C45" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="D45" s="42"/>
+      <c r="D45" s="40"/>
       <c r="F45" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="11" t="s">
@@ -3711,24 +3958,24 @@
         <v>31</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="O45" s="30"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="62"/>
+        <v>187</v>
+      </c>
+      <c r="O45" s="29"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A46" s="61"/>
       <c r="B46" s="11" t="s">
         <v>140</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D46" s="42"/>
+      <c r="D46" s="40"/>
       <c r="F46" s="11" t="s">
         <v>102</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H46" s="11" t="s">
         <v>77</v>
@@ -3739,490 +3986,634 @@
       <c r="J46" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="O46" s="30"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="62"/>
+      <c r="O46" s="29"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A47" s="61"/>
       <c r="B47" s="11" t="s">
         <v>142</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D47" s="42"/>
+      <c r="D47" s="40"/>
       <c r="F47" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I47" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="O47" s="29"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A48" s="61"/>
+      <c r="B48" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="G47" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="I47" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="J47" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="O47" s="30"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="62"/>
-      <c r="B48" s="11" t="s">
+      <c r="C48" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="40"/>
+      <c r="F48" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D48" s="42"/>
-      <c r="F48" s="7" t="s">
-        <v>197</v>
-      </c>
       <c r="G48" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I48" s="44" t="s">
+      <c r="I48" s="42" t="s">
         <v>79</v>
       </c>
       <c r="J48" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O48" s="30"/>
-    </row>
-    <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="62"/>
-      <c r="B49" s="58" t="s">
-        <v>178</v>
-      </c>
-      <c r="C49" s="57" t="s">
+      <c r="O48" s="29"/>
+    </row>
+    <row r="49" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="61"/>
+      <c r="B49" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="D49" s="59"/>
-      <c r="E49" s="57"/>
-      <c r="F49" s="57" t="s">
+      <c r="D49" s="58"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56" t="s">
         <v>28</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="H49" s="56" t="s">
+      <c r="H49" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="I49" s="56" t="s">
+      <c r="I49" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="J49" s="60">
+      <c r="J49" s="59">
         <v>0</v>
       </c>
-      <c r="O49" s="30"/>
-    </row>
-    <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="62"/>
-      <c r="B50" s="58"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
+      <c r="O49" s="29"/>
+    </row>
+    <row r="50" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="61"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
       <c r="G50" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="H50" s="55"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="59"/>
+      <c r="O50" s="29"/>
+    </row>
+    <row r="51" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="61"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="H50" s="56"/>
-      <c r="I50" s="56"/>
-      <c r="J50" s="60"/>
-      <c r="O50" s="30"/>
-    </row>
-    <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="62"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="7" t="s">
+      <c r="H51" s="55"/>
+      <c r="I51" s="55"/>
+      <c r="J51" s="59"/>
+      <c r="O51" s="29"/>
+    </row>
+    <row r="52" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="61"/>
+      <c r="B52" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="C52" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="D52" s="72" t="s">
+        <v>184</v>
+      </c>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="G52" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="H51" s="56"/>
-      <c r="I51" s="56"/>
-      <c r="J51" s="60"/>
-      <c r="O51" s="30"/>
-    </row>
-    <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="62"/>
-      <c r="B52" s="57" t="s">
-        <v>177</v>
-      </c>
-      <c r="C52" s="57" t="s">
-        <v>179</v>
-      </c>
-      <c r="D52" s="74" t="s">
-        <v>185</v>
-      </c>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="G52" s="11" t="s">
+      <c r="H52" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="I52" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="J52" s="56">
+        <v>0</v>
+      </c>
+      <c r="O52" s="29"/>
+    </row>
+    <row r="53" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="61"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="H52" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="I52" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="J52" s="57">
-        <v>0</v>
-      </c>
-      <c r="O52" s="30"/>
-    </row>
-    <row r="53" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="62"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="74"/>
-      <c r="E53" s="57"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="11" t="s">
+      <c r="H53" s="55"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="56"/>
+      <c r="O53" s="29"/>
+    </row>
+    <row r="54" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="61"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="72"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="H53" s="56"/>
-      <c r="I53" s="56"/>
-      <c r="J53" s="57"/>
-      <c r="O53" s="30"/>
-    </row>
-    <row r="54" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="62"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="H54" s="56"/>
-      <c r="I54" s="56"/>
-      <c r="J54" s="57"/>
-      <c r="O54" s="30"/>
-    </row>
-    <row r="55" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="67"/>
+      <c r="H54" s="55"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="56"/>
+      <c r="O54" s="29"/>
+    </row>
+    <row r="55" spans="1:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="65"/>
       <c r="B55" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D55" s="42"/>
+      <c r="D55" s="40"/>
       <c r="F55" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H55" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I55" s="44" t="s">
+      <c r="I55" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="J55" s="31">
+      <c r="J55" s="30">
         <v>0</v>
       </c>
-      <c r="O55" s="30"/>
-    </row>
-    <row r="56" spans="1:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="33" t="s">
+      <c r="O55" s="29"/>
+    </row>
+    <row r="56" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="D56" s="18" t="s">
+      <c r="C56" s="103" t="s">
+        <v>145</v>
+      </c>
+      <c r="D56" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E56" s="18" t="s">
+      <c r="E56" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F56" s="18" t="s">
+      <c r="F56" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G56" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="H56" s="18" t="s">
+      <c r="G56" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="H56" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="I56" s="18" t="s">
+      <c r="I56" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="J56" s="18" t="s">
+      <c r="J56" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="K56" s="18" t="s">
+      <c r="K56" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L56" s="18" t="s">
+      <c r="L56" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="M56" s="18" t="s">
+      <c r="M56" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="N56" s="18" t="s">
+      <c r="N56" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="O56" s="19" t="s">
+      <c r="O56" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="63" t="s">
+    <row r="57" spans="1:18" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="114" t="s">
+        <v>281</v>
+      </c>
+      <c r="B57" s="101" t="s">
+        <v>245</v>
+      </c>
+      <c r="C57" s="27"/>
+      <c r="D57" s="94" t="s">
+        <v>263</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="I57" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K57" s="27"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="109" t="s">
+        <v>260</v>
+      </c>
+      <c r="N57" s="109" t="s">
+        <v>261</v>
+      </c>
+      <c r="O57" s="28"/>
+      <c r="P57" s="112" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q57" s="113"/>
+      <c r="R57" s="88" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="62"/>
+      <c r="B58" s="101" t="s">
+        <v>246</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58" s="94" t="s">
+        <v>247</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G58" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J58" s="7">
+        <v>0</v>
+      </c>
+      <c r="M58" s="93" t="s">
+        <v>265</v>
+      </c>
+      <c r="N58" s="93" t="s">
+        <v>265</v>
+      </c>
+      <c r="O58" s="29"/>
+      <c r="P58" s="112"/>
+      <c r="Q58" s="113"/>
+      <c r="R58" s="88"/>
+    </row>
+    <row r="59" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="62"/>
+      <c r="B59" s="101" t="s">
+        <v>248</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59" s="94" t="s">
+        <v>270</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="G59" s="111" t="s">
+        <v>271</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J59" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="M59" s="110" t="s">
+        <v>278</v>
+      </c>
+      <c r="N59" s="56"/>
+      <c r="O59" s="29"/>
+      <c r="P59" s="112"/>
+      <c r="Q59" s="113"/>
+      <c r="R59" s="88"/>
+    </row>
+    <row r="60" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="62"/>
+      <c r="B60" s="101" t="s">
+        <v>249</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60" s="94" t="s">
+        <v>247</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="G60" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="M60" s="93" t="s">
+        <v>265</v>
+      </c>
+      <c r="N60" s="93" t="s">
+        <v>265</v>
+      </c>
+      <c r="O60" s="29"/>
+      <c r="P60" s="112"/>
+      <c r="Q60" s="113"/>
+      <c r="R60" s="88"/>
+    </row>
+    <row r="61" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="62"/>
+      <c r="B61" s="108" t="s">
+        <v>250</v>
+      </c>
+      <c r="C61" s="107"/>
+      <c r="D61" s="106" t="s">
+        <v>251</v>
+      </c>
+      <c r="E61" s="104" t="s">
+        <v>259</v>
+      </c>
+      <c r="F61" s="104"/>
+      <c r="G61" s="104"/>
+      <c r="H61" s="104"/>
+      <c r="I61" s="104"/>
+      <c r="J61" s="104"/>
+      <c r="K61" s="104"/>
+      <c r="L61" s="104"/>
+      <c r="M61" s="104"/>
+      <c r="N61" s="104"/>
+      <c r="O61" s="105"/>
+      <c r="P61" s="112"/>
+      <c r="Q61" s="113"/>
+      <c r="R61" s="88"/>
+    </row>
+    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="62"/>
+      <c r="B62" s="101" t="s">
+        <v>252</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62" s="94" t="s">
+        <v>253</v>
+      </c>
+      <c r="F62" s="46" t="s">
+        <v>287</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H62" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J62" s="94" t="s">
+        <v>290</v>
+      </c>
+      <c r="M62" s="74" t="s">
+        <v>288</v>
+      </c>
+      <c r="N62" s="74" t="s">
+        <v>289</v>
+      </c>
+      <c r="O62" s="29"/>
+      <c r="P62" s="112"/>
+      <c r="Q62" s="113"/>
+      <c r="R62" s="88"/>
+    </row>
+    <row r="63" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="62"/>
+      <c r="B63" s="108" t="s">
+        <v>254</v>
+      </c>
+      <c r="C63" s="107"/>
+      <c r="D63" s="106" t="s">
+        <v>255</v>
+      </c>
+      <c r="E63" s="104" t="s">
+        <v>259</v>
+      </c>
+      <c r="F63" s="104"/>
+      <c r="G63" s="104"/>
+      <c r="H63" s="104"/>
+      <c r="I63" s="104"/>
+      <c r="J63" s="104"/>
+      <c r="K63" s="104"/>
+      <c r="L63" s="104"/>
+      <c r="M63" s="104"/>
+      <c r="N63" s="104"/>
+      <c r="O63" s="105"/>
+      <c r="P63" s="112"/>
+      <c r="Q63" s="113"/>
+      <c r="R63" s="88"/>
+    </row>
+    <row r="64" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="62"/>
+      <c r="B64" s="101" t="s">
+        <v>256</v>
+      </c>
+      <c r="C64"/>
+      <c r="D64" s="94" t="s">
+        <v>280</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J64" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="O64" s="29"/>
+      <c r="P64" s="112"/>
+      <c r="Q64" s="113"/>
+      <c r="R64" s="88"/>
+    </row>
+    <row r="65" spans="1:18" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="62"/>
+      <c r="B65" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="C65"/>
+      <c r="D65" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="G65" s="111" t="s">
+        <v>284</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J65" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="M65" s="115" t="s">
+        <v>282</v>
+      </c>
+      <c r="N65" s="115" t="s">
+        <v>283</v>
+      </c>
+      <c r="O65" s="29"/>
+      <c r="P65" s="112"/>
+      <c r="Q65" s="113"/>
+      <c r="R65" s="88"/>
+    </row>
+    <row r="66" spans="1:18" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="103" t="s">
         <v>145</v>
       </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="28"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="28"/>
-      <c r="L57" s="28"/>
-      <c r="M57" s="28"/>
-      <c r="N57" s="28"/>
-      <c r="O57" s="29"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="64"/>
-      <c r="B58" s="11"/>
-      <c r="D58" s="13"/>
-      <c r="G58" s="7"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="7"/>
-      <c r="O58" s="30"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="64"/>
-      <c r="B59" s="11"/>
-      <c r="D59" s="13"/>
-      <c r="G59" s="7"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="7"/>
-      <c r="O59" s="30"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="64"/>
-      <c r="B60" s="11"/>
-      <c r="D60" s="13"/>
-      <c r="G60" s="7"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="7"/>
-      <c r="O60" s="30"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="64"/>
-      <c r="B61" s="11"/>
-      <c r="D61" s="13"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="7"/>
-      <c r="O61" s="30"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="64"/>
-      <c r="B62" s="11"/>
-      <c r="D62" s="9"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="7"/>
-      <c r="O62" s="30"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="64"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
-      <c r="N63" s="13"/>
-      <c r="O63" s="37"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="64"/>
-      <c r="B64" s="11"/>
-      <c r="D64" s="10"/>
-      <c r="G64" s="7"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="7"/>
-      <c r="O64" s="30"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="64"/>
-      <c r="B65" s="11"/>
-      <c r="D65" s="10"/>
-      <c r="G65" s="7"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="7"/>
-      <c r="O65" s="30"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="64"/>
-      <c r="B66" s="11"/>
-      <c r="D66" s="10"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="I66" s="12"/>
-      <c r="J66" s="7"/>
-      <c r="O66" s="30"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="64"/>
-      <c r="B67" s="39"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="42"/>
-      <c r="F67" s="7"/>
+      <c r="D66" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="H66" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="I66" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="J66" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="K66" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L66" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M66" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N66" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="O66" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="46"/>
+      <c r="D67" s="13"/>
       <c r="G67" s="7"/>
       <c r="I67" s="12"/>
       <c r="J67" s="7"/>
-      <c r="O67" s="30"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="64"/>
-      <c r="B68" s="39"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="42"/>
-      <c r="F68" s="7"/>
+      <c r="O67" s="27"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B68" s="46"/>
+      <c r="D68" s="13"/>
       <c r="G68" s="7"/>
+      <c r="I68" s="12"/>
       <c r="J68" s="7"/>
-      <c r="O68" s="30"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="64"/>
-      <c r="B69" s="39"/>
-      <c r="C69" s="39"/>
-      <c r="D69" s="42"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="7"/>
-      <c r="O69" s="30"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="64"/>
-      <c r="B70" s="11"/>
-      <c r="D70" s="42"/>
-      <c r="G70" s="7"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="7"/>
-      <c r="O70" s="30"/>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="64"/>
-      <c r="B71" s="11"/>
-      <c r="D71" s="42"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="J71" s="7"/>
-      <c r="O71" s="30"/>
-    </row>
-    <row r="72" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="64"/>
-      <c r="B72" s="11"/>
-      <c r="D72" s="16"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="7"/>
-      <c r="O72" s="30"/>
-    </row>
-    <row r="73" spans="1:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B73" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C73" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E73" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F73" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G73" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="H73" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I73" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="J73" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K73" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="L73" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="M73" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="N73" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="O73" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="11"/>
-      <c r="D74" s="13"/>
-      <c r="G74" s="7"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="7"/>
-      <c r="O74" s="28"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="11"/>
-      <c r="D75" s="13"/>
-      <c r="G75" s="7"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="41">
+    <mergeCell ref="P57:Q65"/>
+    <mergeCell ref="R57:R65"/>
+    <mergeCell ref="E61:O61"/>
+    <mergeCell ref="E63:O63"/>
+    <mergeCell ref="M59:N59"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="A28:A55"/>
     <mergeCell ref="P8:P26"/>
     <mergeCell ref="Q8:Q26"/>
     <mergeCell ref="M10:N13"/>
     <mergeCell ref="R8:R26"/>
-    <mergeCell ref="A57:A72"/>
+    <mergeCell ref="A57:A65"/>
     <mergeCell ref="R3:U3"/>
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="D25:D26"/>
@@ -4261,12 +4652,21 @@
     <hyperlink ref="B6" r:id="rId5" tooltip="Higgs® 10" display="https://www.alientechnology.com/ic/higgs-10/"/>
     <hyperlink ref="A2:A6" r:id="rId6" display="Alien"/>
     <hyperlink ref="A8:A26" r:id="rId7" display="IMPINJ"/>
-    <hyperlink ref="A57:A72" r:id="rId8" display="EM Microelectronic"/>
+    <hyperlink ref="A57:A65" r:id="rId8" display="EM Microelectronic"/>
     <hyperlink ref="R4" r:id="rId9"/>
+    <hyperlink ref="B57" r:id="rId10" display="https://www.emmicroelectronic.com/zh-hans/node/409"/>
+    <hyperlink ref="B58" r:id="rId11" display="https://www.emmicroelectronic.com/zh-hans/node/53"/>
+    <hyperlink ref="B59" r:id="rId12" display="https://www.emmicroelectronic.com/zh-hans/node/52"/>
+    <hyperlink ref="B60" r:id="rId13" display="https://www.emmicroelectronic.com/zh-hans/node/57"/>
+    <hyperlink ref="B61" r:id="rId14" display="https://www.emmicroelectronic.com/zh-hans/node/318"/>
+    <hyperlink ref="B62" r:id="rId15" display="https://www.emmicroelectronic.com/zh-hans/node/317"/>
+    <hyperlink ref="B63" r:id="rId16" display="https://www.emmicroelectronic.com/zh-hans/node/110"/>
+    <hyperlink ref="B64" r:id="rId17" display="https://www.emmicroelectronic.com/index.php/zh-hans/node/444"/>
+    <hyperlink ref="B65" r:id="rId18" display="https://www.emmicroelectronic.com/index.php/zh-hans/node/428"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
-  <legacyDrawing r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -4285,12 +4685,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
-        <v>164</v>
+      <c r="A8" s="41" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>